<commit_message>
Fix some broken links and formatting errors.
</commit_message>
<xml_diff>
--- a/Bare-vs-Coated-Water-Pipelines.xlsx
+++ b/Bare-vs-Coated-Water-Pipelines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igna/Dropbox/Victaulic/FBE_vs_Bare/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E418DE27-9315-3145-8246-96F757045E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D044B3E-6C74-7B4F-BFAD-E936A73E3149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32860" yWindow="760" windowWidth="32860" windowHeight="21580" xr2:uid="{4A80D9CF-9772-3D47-BAD7-B0FB3ABE71DF}"/>
+    <workbookView xWindow="-32840" yWindow="760" windowWidth="32860" windowHeight="21580" activeTab="1" xr2:uid="{4A80D9CF-9772-3D47-BAD7-B0FB3ABE71DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="9" r:id="rId1"/>
@@ -219,7 +219,13 @@
     <definedName name="solver_typ" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="9" hidden="1">2</definedName>
-    <definedName name="Steel_cost_difference">Steel!$E$32</definedName>
+    <definedName name="Steel_a1">Steel!$C$32</definedName>
+    <definedName name="Steel_a2">Steel!$C$33</definedName>
+    <definedName name="Steel_b1">Steel!$D$32</definedName>
+    <definedName name="Steel_b2">Steel!$D$33</definedName>
+    <definedName name="Steel_c1">Steel!$C$34</definedName>
+    <definedName name="Steel_c2">Steel!$D$34</definedName>
+    <definedName name="Steel_cost_difference">Steel!$E$34</definedName>
     <definedName name="Steel_density_kg_m3">Data_!$C$6</definedName>
     <definedName name="Steel_diff_percentage">Steel!$E$33</definedName>
     <definedName name="Steel_pipe_transportation">Data_!$C$77</definedName>
@@ -497,7 +503,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="399">
   <si>
     <t>FBE Coated Case</t>
   </si>
@@ -1741,6 +1747,9 @@
   </si>
   <si>
     <t>Steel Weight</t>
+  </si>
+  <si>
+    <t>Coated</t>
   </si>
 </sst>
 </file>
@@ -2505,7 +2514,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="13" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="331">
+  <cellXfs count="330">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3130,7 +3139,6 @@
     <xf numFmtId="194" fontId="31" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="44" fillId="13" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3981,7 +3989,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Steel!$B$32</c:f>
+              <c:f>Steel!$B$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4156,25 +4164,25 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>FBE</c:v>
+                  <c:v>Bare</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bare</c:v>
+                  <c:v>Coated</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Steel!$C$32:$D$32</c:f>
+              <c:f>Steel!$C$34:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16391991.608976576</c:v>
+                  <c:v>22720068.308931705</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22720068.308931705</c:v>
+                  <c:v>16391991.608976576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16050,7 +16058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401804B6-E255-0D47-B4C0-0EFB54D89CFA}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
@@ -16109,7 +16117,7 @@
       <c r="B4" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="322">
+      <c r="C4" s="321">
         <f>pipeline_length/1000</f>
         <v>70</v>
       </c>
@@ -16571,7 +16579,7 @@
       <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="321">
+      <c r="C26" s="320">
         <v>82</v>
       </c>
       <c r="D26" t="s">
@@ -16790,9 +16798,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:56">
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
+      <c r="B1" s="323"/>
+      <c r="C1" s="323"/>
+      <c r="D1" s="323"/>
       <c r="E1" s="115"/>
       <c r="F1" s="2"/>
       <c r="H1" s="2" t="e">
@@ -18144,10 +18152,10 @@
         <v>#NAME?</v>
       </c>
       <c r="AO19" s="2"/>
-      <c r="AQ19" s="325" t="s">
+      <c r="AQ19" s="324" t="s">
         <v>39</v>
       </c>
-      <c r="AR19" s="325"/>
+      <c r="AR19" s="324"/>
     </row>
     <row r="20" spans="2:52">
       <c r="B20" s="106" t="s">
@@ -18320,7 +18328,7 @@
       <c r="AG21" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AO21" s="326" t="s">
+      <c r="AO21" s="325" t="s">
         <v>12</v>
       </c>
       <c r="AP21" s="14" t="s">
@@ -18413,7 +18421,7 @@
       <c r="AE22" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AO22" s="327"/>
+      <c r="AO22" s="326"/>
       <c r="AP22" s="18" t="s">
         <v>46</v>
       </c>
@@ -18505,7 +18513,7 @@
         <f>Table5[[#This Row],[Friction Head Loss]]</f>
         <v>#NAME?</v>
       </c>
-      <c r="AO23" s="328"/>
+      <c r="AO23" s="327"/>
       <c r="AP23" s="18" t="s">
         <v>47</v>
       </c>
@@ -18672,7 +18680,7 @@
         <f>Table5[[#This Row],[Friction Head Loss]]</f>
         <v>#NAME?</v>
       </c>
-      <c r="AO25" s="329" t="s">
+      <c r="AO25" s="328" t="s">
         <v>48</v>
       </c>
       <c r="AP25" s="20" t="s">
@@ -18759,7 +18767,7 @@
         <f>Table5[[#This Row],[Friction Head Loss]]</f>
         <v>#NAME?</v>
       </c>
-      <c r="AO26" s="329"/>
+      <c r="AO26" s="328"/>
       <c r="AP26" s="24" t="s">
         <v>52</v>
       </c>
@@ -18868,7 +18876,7 @@
         <f>Table5[[#This Row],[Friction Head Loss]]</f>
         <v>#NAME?</v>
       </c>
-      <c r="AO27" s="329"/>
+      <c r="AO27" s="328"/>
       <c r="AP27" s="28" t="s">
         <v>55</v>
       </c>
@@ -18980,7 +18988,7 @@
         <f>Table5[[#This Row],[Friction Head Loss]]</f>
         <v>#NAME?</v>
       </c>
-      <c r="AO28" s="329"/>
+      <c r="AO28" s="328"/>
       <c r="AP28" s="30" t="s">
         <v>58</v>
       </c>
@@ -21005,7 +21013,7 @@
       <c r="D63" s="107" t="s">
         <v>132</v>
       </c>
-      <c r="G63" s="330" t="s">
+      <c r="G63" s="329" t="s">
         <v>162</v>
       </c>
       <c r="H63" s="93" t="s">
@@ -21028,7 +21036,7 @@
         <f>FBE_coating_capex/1000000/FBE_steel_capex</f>
         <v>#NAME?</v>
       </c>
-      <c r="G64" s="330"/>
+      <c r="G64" s="329"/>
       <c r="H64" s="91" t="s">
         <v>172</v>
       </c>
@@ -21038,7 +21046,7 @@
       </c>
     </row>
     <row r="65" spans="2:10">
-      <c r="G65" s="330"/>
+      <c r="G65" s="329"/>
       <c r="H65" s="91" t="s">
         <v>46</v>
       </c>
@@ -21054,7 +21062,7 @@
       <c r="C66" s="134" t="s">
         <v>135</v>
       </c>
-      <c r="G66" s="323" t="s">
+      <c r="G66" s="322" t="s">
         <v>163</v>
       </c>
       <c r="H66" s="91" t="s">
@@ -21076,7 +21084,7 @@
       <c r="D67" s="135">
         <v>2.3478260869565216E-2</v>
       </c>
-      <c r="G67" s="323"/>
+      <c r="G67" s="322"/>
       <c r="H67" s="95" t="s">
         <v>172</v>
       </c>
@@ -22225,9 +22233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A178BA-5E80-3042-B3AF-9144313DE68D}">
   <dimension ref="B2:F39"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22600,10 +22608,10 @@
     </row>
     <row r="31" spans="2:6">
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>398</v>
       </c>
       <c r="E31" t="s">
         <v>39</v>
@@ -22614,54 +22622,48 @@
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="167" t="s">
-        <v>330</v>
-      </c>
-      <c r="C32" s="162">
-        <f>C28</f>
-        <v>16391991.608976576</v>
-      </c>
-      <c r="D32" s="162">
-        <f>C18</f>
-        <v>22720068.308931705</v>
-      </c>
-      <c r="E32" s="162">
-        <f>D32-C32</f>
-        <v>6328076.6999551281</v>
+        <v>396</v>
+      </c>
+      <c r="C32">
+        <f>bare_wall__yr_1_mm</f>
+        <v>13.28</v>
+      </c>
+      <c r="D32">
+        <f>C23</f>
+        <v>9.5299999999999994</v>
       </c>
       <c r="F32" s="164">
-        <f>1-C32/D32</f>
-        <v>0.27852366524212591</v>
+        <f>1-C34/D34</f>
+        <v>-0.38604684841894077</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="167" t="s">
         <v>397</v>
       </c>
-      <c r="C33" s="320">
-        <f>C27/1000</f>
+      <c r="C33" s="236">
+        <f>bare_steel_weight_t</f>
+        <v>16000.048104881484</v>
+      </c>
+      <c r="D33" s="236">
+        <f>fbe_steel_weight_t</f>
         <v>11543.656062659562</v>
       </c>
-      <c r="D33" s="320">
-        <f>capex_steel_fbe/1000</f>
-        <v>16391.991608976576</v>
-      </c>
-      <c r="E33" s="164">
-        <f>(D33-C33)/D33</f>
-        <v>0.29577464788732383</v>
-      </c>
+      <c r="E33" s="164"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="167" t="s">
-        <v>396</v>
-      </c>
-      <c r="C34">
-        <f>bare_wall__yr_1_mm</f>
-        <v>13.28</v>
-      </c>
-      <c r="D34">
-        <f>C23</f>
-        <v>9.5299999999999994</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="C34" s="162">
+        <f>capex_steel_bare</f>
+        <v>22720068.308931705</v>
+      </c>
+      <c r="D34" s="162">
+        <f>capex_steel_fbe</f>
+        <v>16391991.608976576</v>
+      </c>
+      <c r="E34" s="162"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="240" t="s">

</xml_diff>

<commit_message>
Added DOI via Zenodo
</commit_message>
<xml_diff>
--- a/Bare-vs-Coated-Water-Pipelines.xlsx
+++ b/Bare-vs-Coated-Water-Pipelines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igna/Dropbox/Victaulic/FBE_vs_Bare/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D044B3E-6C74-7B4F-BFAD-E936A73E3149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C57F74-4103-EC43-A432-AF8452FED660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32840" yWindow="760" windowWidth="32860" windowHeight="21580" activeTab="1" xr2:uid="{4A80D9CF-9772-3D47-BAD7-B0FB3ABE71DF}"/>
+    <workbookView xWindow="-32860" yWindow="760" windowWidth="32860" windowHeight="21580" xr2:uid="{4A80D9CF-9772-3D47-BAD7-B0FB3ABE71DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="9" r:id="rId1"/>
@@ -32,6 +32,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Charts!$D$1:$G$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parameters!$A$2:$F$25</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">SC!$A$6:$A$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">SC!$B$6:$B$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">SC!$A$6:$A$7</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">SC!$B$6:$B$7</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">SC!$A$6:$A$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">SC!$B$6:$B$7</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">SC!$A$6:$A$7</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">SC!$B$6:$B$7</definedName>
     <definedName name="aguasin_price_200_L_s">Data_!$F$108</definedName>
     <definedName name="annual_discount_rate">Parameters!$C$29</definedName>
     <definedName name="annual_discount_rate_percent">Parameters!$C$28</definedName>
@@ -55,8 +63,8 @@
     <definedName name="bare_re_yr_1">Electricity!$R$22</definedName>
     <definedName name="bare_roughness_yr_1">Electricity!$Q$22</definedName>
     <definedName name="bare_steel_capex">Data_!$C$38</definedName>
-    <definedName name="bare_steel_percentage">Steel!$D$37</definedName>
-    <definedName name="bare_steel_weight_t">Steel!$C$16</definedName>
+    <definedName name="bare_steel_percentage">Steel!$D$38</definedName>
+    <definedName name="bare_steel_weight_t">Steel!$C$17</definedName>
     <definedName name="bare_total_usd">Charts!$E$10</definedName>
     <definedName name="bare_vel_yr_1_m_s">Electricity!$E$22</definedName>
     <definedName name="bare_wall__yr_1_mm">Parameters!$C$11</definedName>
@@ -64,8 +72,8 @@
     <definedName name="biocide_cost_yr">Inhibitors!$F$12</definedName>
     <definedName name="biocide_kg_yr">Inhibitors!$D$12</definedName>
     <definedName name="biocide_price">Inhibitors!$E$12</definedName>
-    <definedName name="capex_steel_bare">Steel!$C$18</definedName>
-    <definedName name="capex_steel_fbe">Steel!$C$28</definedName>
+    <definedName name="capex_steel_bare">Steel!$C$19</definedName>
+    <definedName name="capex_steel_fbe">Steel!$C$29</definedName>
     <definedName name="case_selection">Electricity!$B$18</definedName>
     <definedName name="case_selection_2">Electricity!$J$18</definedName>
     <definedName name="chem_inj_1">Data_!$D$83</definedName>
@@ -84,6 +92,7 @@
     <definedName name="corrosion_rate_mm_yr">Data_!$C$9</definedName>
     <definedName name="cost_of_steel_MT">Data_!#REF!</definedName>
     <definedName name="cost_per_steel_weight">Steel!$C$13</definedName>
+    <definedName name="cost_per_steel_weight_t">Steel!$C$14</definedName>
     <definedName name="design_flow_rate">Parameters!$C$15</definedName>
     <definedName name="design_flow_rate_l_s">Parameters!$C$14</definedName>
     <definedName name="diameter_mm">Data_!$C$28</definedName>
@@ -134,11 +143,12 @@
     <definedName name="fbe_inspections_PV">Inspections!$C$8</definedName>
     <definedName name="FBE_opex_NPV">Table5[[#Totals],[OPEX]]</definedName>
     <definedName name="FBE_opex_NPV_1">Table5[[#Totals],[OPEX]]</definedName>
+    <definedName name="FBE_plus_bare">SC!$B$8</definedName>
     <definedName name="FBE_re_yr_1">#REF!</definedName>
     <definedName name="FBE_steel_capex">Data_!$C$50</definedName>
-    <definedName name="FBE_steel_percentage">Steel!$D$38</definedName>
-    <definedName name="FBE_Steel_Perecentage">SC!$B$8</definedName>
-    <definedName name="fbe_steel_weight_t">Steel!$C$26</definedName>
+    <definedName name="FBE_steel_percentage">Steel!$D$39</definedName>
+    <definedName name="FBE_Steel_Perecentage">SC!$B$9</definedName>
+    <definedName name="fbe_steel_weight_t">Steel!$C$27</definedName>
     <definedName name="fbe_total_usd">Charts!$F$10</definedName>
     <definedName name="fbe_wall__yr_1_mm">Parameters!$C$10</definedName>
     <definedName name="FBE_wall_yr_1">#REF!</definedName>
@@ -219,15 +229,16 @@
     <definedName name="solver_typ" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="9" hidden="1">2</definedName>
-    <definedName name="Steel_a1">Steel!$C$32</definedName>
-    <definedName name="Steel_a2">Steel!$C$33</definedName>
-    <definedName name="Steel_b1">Steel!$D$32</definedName>
-    <definedName name="Steel_b2">Steel!$D$33</definedName>
-    <definedName name="Steel_c1">Steel!$C$34</definedName>
-    <definedName name="Steel_c2">Steel!$D$34</definedName>
-    <definedName name="Steel_cost_difference">Steel!$E$34</definedName>
+    <definedName name="Steel_a1">Steel!$C$33</definedName>
+    <definedName name="Steel_a2">Steel!$C$34</definedName>
+    <definedName name="Steel_b1">Steel!$D$33</definedName>
+    <definedName name="Steel_b2">Steel!$D$34</definedName>
+    <definedName name="Steel_c1">Steel!$C$35</definedName>
+    <definedName name="Steel_c2">Steel!$D$35</definedName>
+    <definedName name="Steel_cost_difference">Steel!$E$35</definedName>
     <definedName name="Steel_density_kg_m3">Data_!$C$6</definedName>
-    <definedName name="Steel_diff_percentage">Steel!$E$33</definedName>
+    <definedName name="Steel_diff_percentage">Steel!$E$34</definedName>
+    <definedName name="Steel_Perecentage">SC!$B$10</definedName>
     <definedName name="Steel_pipe_transportation">Data_!$C$77</definedName>
     <definedName name="Steel_price_USD_MT">Data_!#REF!</definedName>
     <definedName name="Supply_contingency">Data_!$C$34</definedName>
@@ -237,8 +248,8 @@
     <definedName name="Utilization_factor">Data_!#REF!</definedName>
     <definedName name="v_kinematic_viscosity">Data_!$C$30</definedName>
     <definedName name="viscosity_Pa_s">Data_!$C$15</definedName>
-    <definedName name="volume_1_m_bare">Steel!$C$15</definedName>
-    <definedName name="volume_1_m_fbe">Steel!$C$25</definedName>
+    <definedName name="volume_1_m_bare">Steel!$C$16</definedName>
+    <definedName name="volume_1_m_fbe">Steel!$C$26</definedName>
     <definedName name="volume_yr">Inhibitors!$C$6</definedName>
     <definedName name="wall_corrosion_rate_mm_yr">Parameters!$C$9</definedName>
     <definedName name="wall_thickness_corrosion_mm">Data_!#REF!</definedName>
@@ -503,7 +514,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="400">
   <si>
     <t>FBE Coated Case</t>
   </si>
@@ -1359,9 +1370,6 @@
     <t>Extra energy</t>
   </si>
   <si>
-    <t>Shop FBE</t>
-  </si>
-  <si>
     <t>Extra Inspections</t>
   </si>
   <si>
@@ -1674,9 +1682,6 @@
     <t>FBE · Steel weight of pipes</t>
   </si>
   <si>
-    <t>FBE vs Steel Perecentage</t>
-  </si>
-  <si>
     <t>Field Joint Coating</t>
   </si>
   <si>
@@ -1750,6 +1755,15 @@
   </si>
   <si>
     <t>Coated</t>
+  </si>
+  <si>
+    <t>FBE percentage</t>
+  </si>
+  <si>
+    <t>Steel Percentage</t>
+  </si>
+  <si>
+    <t>Interior FBE</t>
   </si>
 </sst>
 </file>
@@ -2514,7 +2528,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="13" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="330">
+  <cellXfs count="332">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3165,6 +3179,8 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="44" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3989,7 +4005,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Steel!$B$34</c:f>
+              <c:f>Steel!$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4057,13 +4073,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.34201927736151722"/>
-                  <c:y val="-1.2358173183230826E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4086,7 +4096,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:dLblPos val="inEnd"/>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4131,7 +4141,7 @@
                 <a:endParaRPr lang="en-CL"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -4160,7 +4170,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Steel!$C$31:$D$31</c:f>
+              <c:f>Steel!$C$32:$D$32</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -4174,7 +4184,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Steel!$C$34:$D$34</c:f>
+              <c:f>Steel!$C$35:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -4209,7 +4219,7 @@
       <c:catAx>
         <c:axId val="836053744"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4251,7 +4261,7 @@
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="0"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -4260,7 +4270,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4350,20 +4360,69 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.7779391315279166E-2"/>
-          <c:y val="0.1229061561408442"/>
-          <c:w val="0.90619576098971022"/>
-          <c:h val="0.86044741112144985"/>
+          <c:x val="7.6206437852210457E-2"/>
+          <c:y val="6.6432702191602444E-3"/>
+          <c:w val="0.90512598470598515"/>
+          <c:h val="0.97671046471177514"/>
         </c:manualLayout>
       </c:layout>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SC!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interior FBE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="76000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="76000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="76000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -4380,8 +4439,288 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk2">
+                            <a:lumMod val="75000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{89D7AFFB-161A-2147-9036-D4AD43B26D1F}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="2000"/>
+                      <a:pPr>
+                        <a:defRPr sz="2000"/>
+                      </a:pPr>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>, </a:t>
+                    </a:r>
+                    <a:fld id="{038151F5-AC2F-8C4A-8FC7-F35C7BB9BF4F}" type="SERIESNAME">
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr sz="2000"/>
+                      </a:pPr>
+                      <a:t>[SERIES NAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" sz="2000" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+              <c:spPr>
+                <a:xfrm>
+                  <a:off x="0" y="1341480"/>
+                  <a:ext cx="2098896" cy="548227"/>
+                </a:xfrm>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:alpha val="67000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="25000"/>
+                      <a:lumOff val="75000"/>
+                      <a:alpha val="67000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:round/>
+                  <a:headEnd type="none" w="med" len="med"/>
+                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:extLst>
+                    <a:ext uri="{C807C97D-BFC1-408E-A445-0C87EB9F89A2}">
+                      <ask:lineSketchStyleProps xmlns:ask="http://schemas.microsoft.com/office/drawing/2018/sketchyshapes" sd="0">
+                        <a:custGeom>
+                          <a:avLst/>
+                          <a:gdLst/>
+                          <a:ahLst/>
+                          <a:cxnLst/>
+                          <a:rect l="0" t="0" r="0" b="0"/>
+                          <a:pathLst/>
+                        </a:custGeom>
+                        <ask:type/>
+                      </ask:lineSketchStyleProps>
+                    </a:ext>
+                  </a:extLst>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk2">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-CL"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst>
+                        <a:gd name="adj1" fmla="val -7934"/>
+                        <a:gd name="adj2" fmla="val -42021"/>
+                      </a:avLst>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.16401066342918169"/>
+                      <c:h val="0.29965729239412747"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C06A-C04B-B648-E44A5EAA0BBC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk2">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>SC!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>761047.67873947392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>SC!$B$9</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>4.4%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C06A-C04B-B648-E44A5EAA0BBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SC!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Steel cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="77000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="77000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="77000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -4395,53 +4734,54 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-C06A-C04B-B648-E44A5EAA0BBC}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.3592704009104868E-4"/>
-                  <c:y val="8.4925152708811066E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.4702557625179542"/>
-                      <c:h val="0.21863075091336881"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-C06A-C04B-B648-E44A5EAA0BBC}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.17664596964428894"/>
-                  <c:y val="-0.1924931533718994"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx2"/>
+                        </a:solidFill>
+                        <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{1928784E-77C8-6B46-A436-03C152308E94}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="2000"/>
+                      <a:pPr>
+                        <a:defRPr sz="2000"/>
+                      </a:pPr>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>, </a:t>
+                    </a:r>
+                    <a:fld id="{1E8B898F-3752-C749-A8CD-B4E025DB3455}" type="SERIESNAME">
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr sz="2000"/>
+                      </a:pPr>
+                      <a:t>[SERIES NAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" sz="2000" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="0.0%" sourceLinked="0"/>
               <c:spPr>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:alpha val="67000"/>
+                  </a:sysClr>
+                </a:solidFill>
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -4452,7 +4792,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx2"/>
                       </a:solidFill>
@@ -4464,43 +4804,53 @@
                   <a:endParaRPr lang="en-CL"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.46330436595312235"/>
-                      <c:h val="0.1771691886132736"/>
+                      <c:w val="0.16260095620824344"/>
+                      <c:h val="0.26021420369687409"/>
                     </c:manualLayout>
                   </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-C06A-C04B-B648-E44A5EAA0BBC}"/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
-            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="67000"/>
+                </a:sysClr>
+              </a:solidFill>
               <a:ln>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="dk2">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4510,78 +4860,111 @@
                 <a:endParaRPr lang="en-CL"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>SC!$A$6:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Shop FBE</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Steel cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SC!$B$6:$B$7</c:f>
+              <c:f>SC!$B$7</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>761047.67873947392</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>16391991.608976576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>SC!$B$10</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>95.6%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C06A-C04B-B648-E44A5EAA0BBC}"/>
+              <c16:uniqueId val="{00000005-97BE-EF4E-8703-DC138473C812}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="16"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:overlap val="100"/>
+        <c:axId val="527415615"/>
+        <c:axId val="469377968"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="469377968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="527415615"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="527415615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="469377968"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4602,9 +4985,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -4616,7 +4997,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200">
+        <a:defRPr sz="1800">
           <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -4754,6 +5135,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.28102670755191334"/>
+                  <c:y val="-0.18682628505706442"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -4766,7 +5153,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="bg1"/>
                       </a:solidFill>
@@ -4778,9 +5165,9 @@
                   <a:endParaRPr lang="en-CL"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="ctr"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
@@ -4803,13 +5190,37 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.0704938995159795E-2"/>
-                  <c:y val="-2.0599250936329586E-2"/>
+                  <c:x val="0.20952987362980224"/>
+                  <c:y val="0.1779026217228464"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-CL"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
@@ -4818,8 +5229,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.31106557377049182"/>
-                      <c:h val="0.16048750850377302"/>
+                      <c:w val="0.25231883769701152"/>
+                      <c:h val="0.16048748119968151"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -4838,7 +5249,7 @@
               </c:layout>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
@@ -4867,7 +5278,7 @@
               </c:layout>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
@@ -4898,7 +5309,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4915,7 +5326,7 @@
             </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
@@ -5032,7 +5443,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1800">
+        <a:defRPr sz="2400">
           <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -13485,13 +13896,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>93134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13568,16 +13979,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>102306</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>141816</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2497667</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107951</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>395111</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>702733</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16058,10 +16469,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401804B6-E255-0D47-B4C0-0EFB54D89CFA}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16074,10 +16485,10 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="233" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B2" s="298" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="298" t="s">
         <v>78</v>
@@ -16086,10 +16497,10 @@
         <v>76</v>
       </c>
       <c r="E2" s="233" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F2" s="233" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -16098,7 +16509,7 @@
         <v>pipeline_length</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C3" s="297">
         <v>70000</v>
@@ -16115,7 +16526,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" s="321">
         <f>pipeline_length/1000</f>
@@ -16131,7 +16542,7 @@
         <v>elevation_change</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5" s="297">
         <v>1000</v>
@@ -16152,7 +16563,7 @@
         <v>segment_length</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="297">
         <v>12</v>
@@ -16173,7 +16584,7 @@
         <v>outside_diameter</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" s="297">
         <v>28</v>
@@ -16194,7 +16605,7 @@
         <v>design_flow_rate_m3_s</v>
       </c>
       <c r="B8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C8">
         <f>CONVERT(outside_diameter_inches,"in","m")</f>
@@ -16216,7 +16627,7 @@
         <v>outside_diameter_inches</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C9" s="297">
         <v>0.15</v>
@@ -16237,7 +16648,7 @@
         <v>design_flow_rate_l_s</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C10" s="297">
         <v>9.5299999999999994</v>
@@ -16258,7 +16669,7 @@
         <v>fbe_wall__yr_1_mm</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11">
         <f>fbe_wall__yr_1_mm+wall_corrosion_rate_mm_yr*25</f>
@@ -16280,7 +16691,7 @@
         <v>fbe_inside_diameter_yr_1</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C12">
         <f>outside_diameter-bare_wall__yr_1_mm/1000*2</f>
@@ -16302,7 +16713,7 @@
         <v>#REF!</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13">
         <f>outside_diameter-fbe_wall__yr_1_mm/1000*2</f>
@@ -16367,7 +16778,7 @@
         <v>x70_steel_density</v>
       </c>
       <c r="B16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C16" s="297">
         <v>7850</v>
@@ -16388,7 +16799,7 @@
         <v>fluid_density</v>
       </c>
       <c r="B17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C17" s="297">
         <v>1030</v>
@@ -16430,7 +16841,7 @@
         <v>roughness_bare_yr_1_mm</v>
       </c>
       <c r="B19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" s="297">
         <v>0.1</v>
@@ -16451,7 +16862,7 @@
         <v>roughness_bare_yr_25_mm</v>
       </c>
       <c r="B20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C20" s="297">
         <v>0.3</v>
@@ -16472,7 +16883,7 @@
         <v>roughness_fbe_yr_1_mm</v>
       </c>
       <c r="B21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" s="297">
         <v>0.01</v>
@@ -16493,7 +16904,7 @@
         <v>roughness_fbe_yr_25_mm</v>
       </c>
       <c r="B22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" s="297">
         <v>0.05</v>
@@ -16535,13 +16946,13 @@
         <v>service_life_yr</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C24" s="297">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -16558,7 +16969,7 @@
       <c r="B25" t="s">
         <v>231</v>
       </c>
-      <c r="C25" s="297">
+      <c r="C25" s="331">
         <v>8400</v>
       </c>
       <c r="D25" t="s">
@@ -16659,7 +17070,7 @@
         <v>hrc_price_usd_t</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C30" s="297">
         <v>625</v>
@@ -16680,7 +17091,7 @@
         <v>field_coating_usd_joint</v>
       </c>
       <c r="B31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C31" s="297">
         <f>1150*0.8</f>
@@ -16702,13 +17113,13 @@
         <v>electrical_energy_usd_mwh</v>
       </c>
       <c r="B32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C32" s="297">
         <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -17071,7 +17482,7 @@
     </row>
     <row r="6" spans="2:56">
       <c r="B6" s="106" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C6" s="110">
         <v>7850</v>
@@ -17149,7 +17560,7 @@
     </row>
     <row r="7" spans="2:56">
       <c r="B7" s="106" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" s="107">
         <v>625</v>
@@ -22231,11 +22642,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A178BA-5E80-3042-B3AF-9144313DE68D}">
-  <dimension ref="B2:F39"/>
+  <dimension ref="B2:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22247,7 +22658,7 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="233" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="233" t="s">
         <v>78</v>
@@ -22256,15 +22667,15 @@
         <v>76</v>
       </c>
       <c r="E2" s="233" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F2" s="233" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="236">
         <f>x70_steel_density</f>
@@ -22279,7 +22690,7 @@
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C4">
         <f>bare_wall__yr_1_mm</f>
@@ -22294,7 +22705,7 @@
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5">
         <f>outside_diameter</f>
@@ -22309,7 +22720,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C6" s="236">
         <f>pipeline_length</f>
@@ -22324,14 +22735,14 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" s="235">
         <f>hrc_price_usd_t/1000</f>
         <v>0.625</v>
       </c>
       <c r="D7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -22339,7 +22750,7 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -22353,7 +22764,7 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C9">
         <v>120</v>
@@ -22367,7 +22778,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C10">
         <v>35</v>
@@ -22381,7 +22792,7 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C11">
         <f>SUM(C8:C10)</f>
@@ -22393,14 +22804,14 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C12" s="235">
         <f>SUM(C8:C10)/1000</f>
         <v>0.17</v>
       </c>
       <c r="D12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -22408,14 +22819,14 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C13" s="237">
         <f>(C7*2+C12)</f>
         <v>1.42</v>
       </c>
       <c r="D13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -22423,294 +22834,306 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>368</v>
-      </c>
-      <c r="C14" s="278">
-        <f>bare_inside_diameter_yr_1</f>
-        <v>0.68464000000000003</v>
+        <v>320</v>
+      </c>
+      <c r="C14" s="330">
+        <f>cost_per_steel_weight*1000</f>
+        <v>1420</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
         <v>367</v>
       </c>
-      <c r="C15" s="279">
+      <c r="C15" s="278">
+        <f>bare_inside_diameter_yr_1</f>
+        <v>0.68464000000000003</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" s="279">
         <f>PI()/4*(outside_diameter^2-bare_inside_diameter_yr_1^2)</f>
         <v>2.9117466978856206E-2</v>
       </c>
-      <c r="D15" s="234" t="s">
-        <v>351</v>
-      </c>
-      <c r="E15" t="b">
+      <c r="D16" s="234" t="s">
+        <v>350</v>
+      </c>
+      <c r="E16" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="238" t="s">
-        <v>369</v>
-      </c>
-      <c r="C16" s="236">
-        <f>C17/1000</f>
-        <v>16000.048104881484</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="238" t="s">
-        <v>369</v>
-      </c>
-      <c r="C17" s="239">
+        <v>368</v>
+      </c>
+      <c r="C17" s="236">
+        <f>C18/1000</f>
+        <v>16000.048104881484</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="238" t="s">
+        <v>368</v>
+      </c>
+      <c r="C18" s="239">
         <f>volume_1_m_bare*C3*C6</f>
         <v>16000048.104881484</v>
       </c>
-      <c r="D17" s="238" t="s">
-        <v>319</v>
-      </c>
-      <c r="E17" t="b">
+      <c r="D18" s="238" t="s">
+        <v>318</v>
+      </c>
+      <c r="E18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
-        <v>327</v>
-      </c>
-      <c r="C18" s="163">
-        <f>C13*C17</f>
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="163">
+        <f>C13*C18</f>
         <v>22720068.308931705</v>
       </c>
-      <c r="D18" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="233" t="s">
-        <v>289</v>
-      </c>
-      <c r="C21" s="233" t="s">
+      <c r="D19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="233" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" s="233" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="233" t="s">
+      <c r="D22" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="233" t="s">
-        <v>303</v>
-      </c>
-      <c r="F21" s="233" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
-        <v>293</v>
-      </c>
-      <c r="C22" s="236">
+      <c r="E22" s="233" t="s">
+        <v>302</v>
+      </c>
+      <c r="F22" s="233" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="236">
         <f>x70_steel_density</f>
         <v>7850</v>
       </c>
-      <c r="D22" s="234" t="s">
+      <c r="D23" s="234" t="s">
         <v>22</v>
       </c>
-      <c r="E22" t="b">
+      <c r="E23" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
-      <c r="B23" t="s">
-        <v>328</v>
-      </c>
-      <c r="C23">
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24">
         <f>fbe_wall__yr_1_mm</f>
         <v>9.5299999999999994</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>27</v>
       </c>
-      <c r="E23" t="b">
+      <c r="E24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" t="s">
-        <v>370</v>
-      </c>
-      <c r="C24">
+    <row r="25" spans="2:6">
+      <c r="B25" t="s">
+        <v>369</v>
+      </c>
+      <c r="C25">
         <f>fbe_inside_diameter_yr_1</f>
         <v>0.69214000000000009</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="E24" t="b">
+      <c r="E25" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" t="s">
-        <v>371</v>
-      </c>
-      <c r="C25">
+    <row r="26" spans="2:6">
+      <c r="B26" t="s">
+        <v>370</v>
+      </c>
+      <c r="C26">
         <f>PI()*(outside_diameter^2-fbe_inside_diameter_yr_1^2)/4</f>
         <v>2.1007563353338601E-2</v>
       </c>
-      <c r="D25" s="234" t="s">
-        <v>351</v>
-      </c>
-      <c r="E25" t="b">
+      <c r="D26" s="234" t="s">
+        <v>350</v>
+      </c>
+      <c r="E26" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="238" t="s">
-        <v>372</v>
-      </c>
-      <c r="C26" s="236">
-        <f>C27/1000</f>
-        <v>11543.656062659562</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="238" t="s">
-        <v>372</v>
-      </c>
-      <c r="C27" s="239">
+        <v>371</v>
+      </c>
+      <c r="C27" s="236">
+        <f>C28/1000</f>
+        <v>11543.656062659562</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="238" t="s">
+        <v>371</v>
+      </c>
+      <c r="C28" s="239">
         <f>volume_1_m_fbe*C3*C6</f>
         <v>11543656.062659562</v>
       </c>
-      <c r="D27" s="238" t="s">
-        <v>319</v>
-      </c>
-      <c r="E27" t="b">
+      <c r="D28" s="238" t="s">
+        <v>318</v>
+      </c>
+      <c r="E28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
-      <c r="B28" t="s">
-        <v>329</v>
-      </c>
-      <c r="C28" s="163">
-        <f>C13*C27</f>
+    <row r="29" spans="2:6">
+      <c r="B29" t="s">
+        <v>328</v>
+      </c>
+      <c r="C29" s="163">
+        <f>C13*C28</f>
         <v>16391991.608976576</v>
       </c>
-      <c r="D28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="C31" t="s">
+      <c r="D29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="C32" t="s">
         <v>41</v>
       </c>
-      <c r="D31" t="s">
-        <v>398</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>396</v>
+      </c>
+      <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="F31" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="167" t="s">
-        <v>396</v>
-      </c>
-      <c r="C32">
+      <c r="F32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="167" t="s">
+        <v>394</v>
+      </c>
+      <c r="C33">
         <f>bare_wall__yr_1_mm</f>
         <v>13.28</v>
       </c>
-      <c r="D32">
-        <f>C23</f>
+      <c r="D33">
+        <f>C24</f>
         <v>9.5299999999999994</v>
       </c>
-      <c r="F32" s="164">
-        <f>1-C34/D34</f>
+      <c r="F33" s="164">
+        <f>1-C35/D35</f>
         <v>-0.38604684841894077</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="167" t="s">
-        <v>397</v>
-      </c>
-      <c r="C33" s="236">
+    <row r="34" spans="2:6">
+      <c r="B34" s="167" t="s">
+        <v>395</v>
+      </c>
+      <c r="C34" s="236">
         <f>bare_steel_weight_t</f>
         <v>16000.048104881484</v>
       </c>
-      <c r="D33" s="236">
+      <c r="D34" s="236">
         <f>fbe_steel_weight_t</f>
         <v>11543.656062659562</v>
       </c>
-      <c r="E33" s="164"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="167" t="s">
-        <v>330</v>
-      </c>
-      <c r="C34" s="162">
+      <c r="E34" s="164"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="167" t="s">
+        <v>329</v>
+      </c>
+      <c r="C35" s="162">
         <f>capex_steel_bare</f>
         <v>22720068.308931705</v>
       </c>
-      <c r="D34" s="162">
+      <c r="D35" s="162">
         <f>capex_steel_fbe</f>
         <v>16391991.608976576</v>
       </c>
-      <c r="E34" s="162"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="240" t="s">
+      <c r="E35" s="162"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="240" t="s">
+        <v>331</v>
+      </c>
+      <c r="C37" s="240" t="s">
         <v>332</v>
       </c>
-      <c r="C36" s="240" t="s">
+      <c r="D37" s="240" t="s">
         <v>333</v>
       </c>
-      <c r="D36" s="240" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="240" t="s">
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="240" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="242">
-        <f>C18</f>
+      <c r="C38" s="242">
+        <f>C19</f>
         <v>22720068.308931705</v>
       </c>
-      <c r="D37" s="241">
+      <c r="D38" s="241">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="240" t="s">
+    <row r="39" spans="2:6">
+      <c r="B39" s="240" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="242">
-        <f>C28</f>
+      <c r="C39" s="242">
+        <f>C29</f>
         <v>16391991.608976576</v>
       </c>
-      <c r="D38" s="243">
-        <f>C38/C37</f>
+      <c r="D39" s="243">
+        <f>C39/C38</f>
         <v>0.72147633475787409</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="240" t="s">
+    <row r="40" spans="2:6">
+      <c r="B40" s="240" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="242">
-        <f>C37-C38</f>
+      <c r="C40" s="242">
+        <f>C38-C39</f>
         <v>6328076.6999551281</v>
       </c>
-      <c r="D39" s="243">
-        <f>C39/C37</f>
+      <c r="D40" s="243">
+        <f>C40/C38</f>
         <v>0.27852366524212591</v>
       </c>
     </row>
@@ -22737,7 +23160,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="233" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="233" t="s">
         <v>78</v>
@@ -22746,15 +23169,15 @@
         <v>76</v>
       </c>
       <c r="D1" s="233" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E1" s="233" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B2" s="244">
         <v>4.5</v>
@@ -22765,7 +23188,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B3">
         <f>design_flow_rate_l_s/1000</f>
@@ -22777,19 +23200,19 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4">
         <f>(24 * 60 * 60)</f>
         <v>86400</v>
       </c>
       <c r="C4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B5" s="162">
         <f>Dosing_investment*B3*B4</f>
@@ -22807,20 +23230,20 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" style="246" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="246" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="246" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.33203125" style="246" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="246"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="16">
       <c r="A1" s="233" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="233" t="s">
         <v>78</v>
@@ -22833,19 +23256,19 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="247" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B2" s="254">
         <v>5</v>
       </c>
       <c r="C2" s="246" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I2" s="248"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="276" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="255">
         <f>fbe_inside_diameter_yr_1</f>
@@ -22857,7 +23280,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="276" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B4" s="246">
         <f>pipeline_length</f>
@@ -22869,7 +23292,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="249" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B5" s="256">
         <f>PI()*fbe_inside_diameter_yr_1*pipeline_length</f>
@@ -22881,7 +23304,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="276" t="s">
-        <v>273</v>
+        <v>399</v>
       </c>
       <c r="B6" s="257">
         <f>FBE_cost_per_surface*fbe_inside_surface</f>
@@ -22891,7 +23314,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="276" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="257">
         <f>capex_steel_fbe</f>
@@ -22903,12 +23326,9 @@
       <c r="I7" s="245"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="246" t="s">
-        <v>373</v>
-      </c>
-      <c r="B8" s="280">
-        <f>interior_fbe_capex/B7</f>
-        <v>4.6428017832970903E-2</v>
+      <c r="B8" s="257">
+        <f>SUM(B6:B7)</f>
+        <v>17153039.28771605</v>
       </c>
       <c r="F8" s="249"/>
       <c r="G8" s="245"/>
@@ -22916,12 +23336,26 @@
       <c r="I8" s="245"/>
     </row>
     <row r="9" spans="1:9">
+      <c r="A9" s="276" t="s">
+        <v>397</v>
+      </c>
+      <c r="B9" s="280">
+        <f>interior_fbe_capex/FBE_plus_bare</f>
+        <v>4.4368095121456952E-2</v>
+      </c>
       <c r="F9" s="249"/>
       <c r="G9" s="250"/>
       <c r="H9" s="245"/>
       <c r="I9" s="245"/>
     </row>
     <row r="10" spans="1:9">
+      <c r="A10" s="276" t="s">
+        <v>398</v>
+      </c>
+      <c r="B10" s="280">
+        <f>B7/FBE_plus_bare</f>
+        <v>0.9556319048785431</v>
+      </c>
       <c r="F10" s="251"/>
       <c r="G10" s="252"/>
       <c r="H10" s="245"/>
@@ -22939,8 +23373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DA13A2-911B-9D49-B1C9-9DED1E3BE9CB}">
   <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A33" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22960,7 +23394,7 @@
     </row>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3" s="166">
         <f>C$9*D3</f>
@@ -22972,7 +23406,7 @@
     </row>
     <row r="4" spans="2:7">
       <c r="B4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C4" s="166">
         <f t="shared" ref="C4:C8" si="0">C$9*D4</f>
@@ -22988,7 +23422,7 @@
     </row>
     <row r="5" spans="2:7">
       <c r="B5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C5" s="166">
         <f t="shared" si="0"/>
@@ -23000,7 +23434,7 @@
     </row>
     <row r="6" spans="2:7">
       <c r="B6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C6" s="166">
         <f t="shared" si="0"/>
@@ -23012,7 +23446,7 @@
     </row>
     <row r="7" spans="2:7">
       <c r="B7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C7" s="166">
         <f t="shared" si="0"/>
@@ -23024,7 +23458,7 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="238" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C8" s="262">
         <f t="shared" si="0"/>
@@ -23036,7 +23470,7 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C9" s="166">
         <f>field_coating_usd_joint</f>
@@ -23049,7 +23483,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11">
         <f>pipeline_length</f>
@@ -23058,7 +23492,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C12">
         <f>segment_length</f>
@@ -23067,16 +23501,16 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="238" t="s">
-        <v>349</v>
-      </c>
-      <c r="C13" s="238">
+        <v>348</v>
+      </c>
+      <c r="C13" s="239">
         <f>ROUNDUP(pipeline_length/segment_length,0)</f>
         <v>5834</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C14" s="162">
         <f>C13*C9</f>
@@ -23085,7 +23519,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C18" s="162">
         <f>capex_steel_fbe</f>
@@ -23098,7 +23532,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C19" s="162">
         <f>field_coating_total</f>
@@ -23111,7 +23545,7 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C20" s="162">
         <f>interior_fbe_capex</f>
@@ -23124,7 +23558,7 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C21" s="162">
         <f>Dosage_plant_investment</f>
@@ -23137,7 +23571,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C22" s="162">
         <f>SUM(C18:C20)</f>
@@ -23173,7 +23607,7 @@
   <sheetData>
     <row r="1" spans="2:12">
       <c r="B1" s="233" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C1" s="233" t="s">
         <v>78</v>
@@ -23184,7 +23618,7 @@
     </row>
     <row r="2" spans="2:12">
       <c r="B2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C2">
         <v>0.7</v>
@@ -23195,26 +23629,26 @@
     </row>
     <row r="3" spans="2:12">
       <c r="B3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C3">
         <f>C2*3600</f>
         <v>2520</v>
       </c>
       <c r="D3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C4">
         <f>C3*24*30</f>
         <v>1814400</v>
       </c>
       <c r="D4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -23226,24 +23660,24 @@
         <v>8400</v>
       </c>
       <c r="D5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C6" s="236">
         <f>C5*C3</f>
         <v>21168000</v>
       </c>
       <c r="D6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C7">
         <f>fluid_density</f>
@@ -23263,7 +23697,7 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="264" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C8" s="273">
         <f>annual_discount_rate</f>
@@ -23273,7 +23707,7 @@
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="264" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C9" s="296">
         <v>0.2</v>
@@ -23281,27 +23715,27 @@
     </row>
     <row r="10" spans="2:12" ht="34">
       <c r="B10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D10" s="270" t="s">
+        <v>357</v>
+      </c>
+      <c r="E10" s="270" t="s">
         <v>356</v>
-      </c>
-      <c r="D10" s="270" t="s">
-        <v>358</v>
-      </c>
-      <c r="E10" s="270" t="s">
-        <v>357</v>
       </c>
       <c r="F10" t="s">
         <v>61</v>
       </c>
       <c r="G10" s="270" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C11" s="271">
         <v>26</v>
@@ -23362,7 +23796,7 @@
     </row>
     <row r="15" spans="2:12">
       <c r="E15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F15" s="263">
         <f>-PV(C8,25,Table9[[#Totals],[Total]])</f>
@@ -23395,7 +23829,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="233" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="233" t="s">
         <v>78</v>
@@ -23406,7 +23840,7 @@
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C3" s="162">
         <v>8000</v>
@@ -23417,7 +23851,7 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C4" s="162">
         <v>4000</v>
@@ -23428,7 +23862,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C5" s="162">
         <f>C3*pipeline_length/1000</f>
@@ -23437,7 +23871,7 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C6" s="162">
         <f>C4*pipeline_length/1000</f>
@@ -23446,7 +23880,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C7" s="263">
         <f>-PV(annual_discount_rate,25,C5)</f>
@@ -23455,7 +23889,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C8" s="263">
         <f>-PV(annual_discount_rate,25,C6)</f>
@@ -23516,7 +23950,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="D3" s="174" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E3" s="170">
         <f>pipeline_length</f>
@@ -23528,7 +23962,7 @@
     </row>
     <row r="4" spans="1:24">
       <c r="D4" s="174" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E4" s="170">
         <f>design_flow_rate</f>
@@ -23540,7 +23974,7 @@
     </row>
     <row r="5" spans="1:24">
       <c r="D5" s="174" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E5" s="170">
         <f>fluid_density</f>
@@ -23549,7 +23983,7 @@
     </row>
     <row r="6" spans="1:24">
       <c r="D6" s="174" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E6" s="170">
         <f>Elevation_change</f>
@@ -23577,25 +24011,25 @@
         <v>8400</v>
       </c>
       <c r="F8" s="170" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="16">
       <c r="A9" s="173"/>
       <c r="B9" s="173"/>
       <c r="D9" s="174" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E9" s="289">
         <v>175</v>
       </c>
       <c r="F9" s="170" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="D10" s="174" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E10" s="170">
         <f>Projected_MWh/1000</f>
@@ -23607,19 +24041,19 @@
     </row>
     <row r="11" spans="1:24">
       <c r="D11" s="174" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E11" s="170">
         <f>Projected_kWh/1000</f>
         <v>1.75E-4</v>
       </c>
       <c r="F11" s="170" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="D12" s="174" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E12" s="290">
         <f ca="1">bare_electricity_yr_1+K22</f>
@@ -23801,28 +24235,28 @@
         <v>258</v>
       </c>
       <c r="F21" s="218" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="218" t="s">
         <v>221</v>
       </c>
       <c r="H21" s="218" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I21" s="218" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J21" s="286" t="s">
+        <v>283</v>
+      </c>
+      <c r="K21" s="286" t="s">
         <v>284</v>
-      </c>
-      <c r="K21" s="286" t="s">
-        <v>285</v>
       </c>
       <c r="L21" s="219" t="s">
         <v>227</v>
       </c>
       <c r="M21" s="219" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N21" s="175" t="s">
         <v>259</v>
@@ -26602,16 +27036,16 @@
         <v>221</v>
       </c>
       <c r="H49" s="218" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I49" s="218" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J49" s="295" t="s">
+        <v>283</v>
+      </c>
+      <c r="K49" s="295" t="s">
         <v>284</v>
-      </c>
-      <c r="K49" s="295" t="s">
-        <v>285</v>
       </c>
       <c r="L49" s="219" t="s">
         <v>227</v>
@@ -29142,7 +29576,7 @@
         <v>159</v>
       </c>
       <c r="F1" s="300" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G1" s="300" t="s">
         <v>39</v>
@@ -29157,7 +29591,7 @@
         <v>625</v>
       </c>
       <c r="C2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D2" s="301" t="s">
         <v>167</v>
@@ -29185,7 +29619,7 @@
         <v>625</v>
       </c>
       <c r="C3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D3" s="303" t="s">
         <v>169</v>
@@ -29213,10 +29647,10 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D4" s="303" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E4" s="304"/>
       <c r="F4" s="304">
@@ -29235,10 +29669,10 @@
         <v>1420</v>
       </c>
       <c r="C5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D5" s="305" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="304">
         <f ca="1">bare_friction_energy_PV</f>
@@ -29256,7 +29690,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="305" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E6" s="304">
         <f>bare_elevation_energy_PV</f>
@@ -29271,7 +29705,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="C7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D7" s="305" t="s">
         <v>168</v>
@@ -29292,7 +29726,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="D8" s="303" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E8" s="304"/>
       <c r="F8" s="304">
@@ -29358,7 +29792,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="D13" s="303" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E13" s="304">
         <f>SUM(E3,E9,E7)</f>
@@ -29375,7 +29809,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="D14" s="305" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E14" s="304">
         <f>SUM(E2,E6,E7)</f>
@@ -29430,7 +29864,7 @@
         <v>159</v>
       </c>
       <c r="F17" s="313" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G17" s="313" t="s">
         <v>39</v>
@@ -29439,7 +29873,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="D18" s="310" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E18" s="314">
         <f>pv_inhibitors</f>
@@ -29453,7 +29887,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="D19" s="310" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E19" s="314">
         <f ca="1">G5</f>
@@ -29483,7 +29917,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="D21" s="310" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E21" s="314"/>
       <c r="F21" s="314">
@@ -29497,7 +29931,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="D22" s="310" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E22" s="314">
         <f>extra_inspections</f>
@@ -29511,7 +29945,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="D23" s="310" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E23" s="314"/>
       <c r="F23" s="314">
@@ -29604,7 +30038,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="167" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B47" s="162" t="s">
         <v>159</v>
@@ -29612,7 +30046,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="158" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B48" s="169">
         <f>NPV(discount_rate/100,Electricity!K22:K46)</f>
@@ -29621,7 +30055,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="158" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B49" s="169">
         <f ca="1">NPV(discount_rate/100,Electricity!J22:J46)</f>

</xml_diff>